<commit_message>
20251204 EZCLA almost done
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/Eurozone 300.xlsx
+++ b/GUI + Reviews/202509/Eurozone 300.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\Data input files\Factset Data\Calculation file\202509\202512\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202509/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{7F73D439-CAFF-4CB7-AD32-FE2D2DAB75E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA55FEA7-29F8-483C-A4D9-E09977B17649}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{AA55FEA7-29F8-483C-A4D9-E09977B17649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3224,28 +3224,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C62BB62-41E2-4B44-BD63-DFC11FBEAC65}" name="Universe" displayName="Universe" ref="A1:S301" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C62BB62-41E2-4B44-BD63-DFC11FBEAC65}" name="Universe" displayName="Universe" ref="A1:S301" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:S301" xr:uid="{7C62BB62-41E2-4B44-BD63-DFC11FBEAC65}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{E215F094-97BE-4944-88AF-6E03B27FD7E1}" name="Rank" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{A91E4964-0DFA-4C23-9C32-4C5B7F81E079}" name="Ticker" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{09C61BBF-4A7D-445C-A174-2633C89C4D03}" name="Name" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{A2472CB4-6BAC-4A2A-A7CD-0C0986AFFA63}" name="ISIN" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{52862F4B-863C-44C7-85EC-28DD545EAF94}" name="MIC" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{CA9060AC-1882-4ED3-A92F-F226B2FAB108}" name="NOSH" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{2CFCA56F-E81D-4BB6-95AA-E107AD2EA801}" name="Price" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{B724BE25-F6F2-44D7-880D-281A7204221D}" name="Currency" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{C58A7779-7C0E-4D8A-80BB-1A3B56CDAC1A}" name="12 month aver. turnover EUR" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{96C464E6-4883-4130-8153-D3AA680273F4}" name="20 days aver. turn EUR" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{007E292D-134A-48BF-A792-25AD6AAECFD6}" name="10 days aver. turn EUR" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{8F40393A-8172-46B5-801C-C6DD195B08B4}" name="5 days aver. turn EUR" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{EA764463-63A5-4B5F-A1D4-28595B849551}" name="6 month aver. turnover EUR" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{6A7F90B4-D9B5-48B0-B4F4-D0D8434BD9CD}" name="126 days volatility" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{8FD176E5-A4AD-4105-9F15-8855B3459B1C}" name="100 days volatility" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{29334AF4-219B-454C-9C53-2C5E4BB0FB4B}" name="100 days aver. turn EUR" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{3786DFEC-D1DB-43ED-8937-1DAF377442D5}" name="180 days volatility" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{FB6945E7-B6C3-4AF7-A681-AB7CB1A73445}" name="3 months aver. Turnover EUR" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{EB7D353A-E6FC-4087-8884-A5CA1001B142}" name="3 months aver. Turnover USD" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E215F094-97BE-4944-88AF-6E03B27FD7E1}" name="Rank" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{A91E4964-0DFA-4C23-9C32-4C5B7F81E079}" name="Ticker" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{09C61BBF-4A7D-445C-A174-2633C89C4D03}" name="Name" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A2472CB4-6BAC-4A2A-A7CD-0C0986AFFA63}" name="ISIN" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{52862F4B-863C-44C7-85EC-28DD545EAF94}" name="MIC" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{CA9060AC-1882-4ED3-A92F-F226B2FAB108}" name="NOSH" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{2CFCA56F-E81D-4BB6-95AA-E107AD2EA801}" name="Price" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{B724BE25-F6F2-44D7-880D-281A7204221D}" name="Currency" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{C58A7779-7C0E-4D8A-80BB-1A3B56CDAC1A}" name="12 month aver. turnover EUR" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{96C464E6-4883-4130-8153-D3AA680273F4}" name="20 days aver. turn EUR" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{007E292D-134A-48BF-A792-25AD6AAECFD6}" name="10 days aver. turn EUR" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{8F40393A-8172-46B5-801C-C6DD195B08B4}" name="5 days aver. turn EUR" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{EA764463-63A5-4B5F-A1D4-28595B849551}" name="6 month aver. turnover EUR" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{6A7F90B4-D9B5-48B0-B4F4-D0D8434BD9CD}" name="126 days volatility" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{8FD176E5-A4AD-4105-9F15-8855B3459B1C}" name="100 days volatility" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{29334AF4-219B-454C-9C53-2C5E4BB0FB4B}" name="100 days aver. turn EUR" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{3786DFEC-D1DB-43ED-8937-1DAF377442D5}" name="180 days volatility" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{FB6945E7-B6C3-4AF7-A681-AB7CB1A73445}" name="3 months aver. Turnover EUR" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{EB7D353A-E6FC-4087-8884-A5CA1001B142}" name="3 months aver. Turnover USD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3570,7 +3570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECF2085-3478-42F7-A3CA-E0866A8BCD8A}">
   <dimension ref="A1:S301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>